<commit_message>
add functionnal mapper & reducer for hadoop
</commit_message>
<xml_diff>
--- a/data/output/top_100_cde_lot1.xlsx
+++ b/data/output/top_100_cde_lot1.xlsx
@@ -1051,74 +1051,74 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MAYENNE</t>
+          <t>BAILLEUL</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>26478</v>
+        <v>43869</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>61</t>
         </is>
       </c>
       <c r="D30" t="n">
         <v>12</v>
       </c>
       <c r="E30" t="n">
-        <v>19.2</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BAILLEUL</t>
+          <t>SAINT PIERRE SUR ERVE</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>43869</v>
+        <v>37017</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D31" t="n">
         <v>12</v>
       </c>
       <c r="E31" t="n">
-        <v>16.5</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SAINT PIERRE SUR ERVE</t>
+          <t>RONFEUGERAI</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>37017</v>
+        <v>34461</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>61</t>
         </is>
       </c>
       <c r="D32" t="n">
         <v>12</v>
       </c>
       <c r="E32" t="n">
-        <v>12.8</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>RONFEUGERAI</t>
+          <t>ST GERMAIN DU CORBEIS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>34461</v>
+        <v>45704</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1126,20 +1126,20 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E33" t="n">
-        <v>10.4</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ST GERMAIN DU CORBEIS</t>
+          <t>VALFRAMBERT</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>45704</v>
+        <v>48801</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1150,38 +1150,38 @@
         <v>11</v>
       </c>
       <c r="E34" t="n">
-        <v>45.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>VALFRAMBERT</t>
+          <t>LE BOURGNEUF LA FORET</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>48801</v>
+        <v>48399</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D35" t="n">
         <v>11</v>
       </c>
       <c r="E35" t="n">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LE BOURGNEUF LA FORET</t>
+          <t>ERNEE</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>48399</v>
+        <v>48720</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1192,38 +1192,38 @@
         <v>11</v>
       </c>
       <c r="E36" t="n">
-        <v>32.5</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ERNEE</t>
+          <t>COLOMBIERS</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>48720</v>
+        <v>47698</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>61</t>
         </is>
       </c>
       <c r="D37" t="n">
         <v>11</v>
       </c>
       <c r="E37" t="n">
-        <v>21.3</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>COLOMBIERS</t>
+          <t>LONLAY L'ABBAYE</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>47698</v>
+        <v>43587</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1234,21 +1234,21 @@
         <v>11</v>
       </c>
       <c r="E38" t="n">
-        <v>19.5</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LONLAY L'ABBAYE</t>
+          <t>SAINT PIERRE DES NIDS</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>43587</v>
+        <v>28924</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1261,32 +1261,32 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SAINT PIERRE DES NIDS</t>
+          <t>AVRILLY</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>28924</v>
+        <v>45147</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>61</t>
         </is>
       </c>
       <c r="D40" t="n">
         <v>11</v>
       </c>
       <c r="E40" t="n">
-        <v>19.2</v>
+        <v>17.7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AVRILLY</t>
+          <t>BOISSY MAUGIS</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>45147</v>
+        <v>43918</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1297,17 +1297,17 @@
         <v>11</v>
       </c>
       <c r="E41" t="n">
-        <v>17.7</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BOISSY MAUGIS</t>
+          <t>LA FERRIERE AUX ETANGS</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>43918</v>
+        <v>39237</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1318,17 +1318,17 @@
         <v>11</v>
       </c>
       <c r="E42" t="n">
-        <v>16.5</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>LA FERRIERE AUX ETANGS</t>
+          <t>ATHIS VAL DE ROUVRE</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>39237</v>
+        <v>36300</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1339,21 +1339,21 @@
         <v>11</v>
       </c>
       <c r="E43" t="n">
-        <v>15.4</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ATHIS VAL DE ROUVRE</t>
+          <t>MAYENNE</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>36300</v>
+        <v>26478</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D44" t="n">

</xml_diff>